<commit_message>
Excercise-NotView: Progress in the lofic of the sequence
</commit_message>
<xml_diff>
--- a/DataTable manipulation/Sample Columns - Notview.xlsx
+++ b/DataTable manipulation/Sample Columns - Notview.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF2780D-0593-4D2C-BC45-114FBF435013}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF39D8-8D78-4570-9D89-82DB4CF05461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6585" yWindow="2790" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -56,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,99 +381,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>159</v>
+        <v>3359</v>
       </c>
       <c r="B1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3359</v>
+        <v>9072</v>
       </c>
       <c r="B2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8996</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9072</v>
+        <v>623</v>
       </c>
       <c r="B3">
-        <v>8996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>623</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11</v>
+        <v>6643</v>
       </c>
       <c r="B5">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>88942</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6643</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>88942</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>3213</v>
       </c>
       <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4324</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3213</v>
+        <v>7732</v>
       </c>
       <c r="B8">
-        <v>4324</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7732</v>
+        <v>952</v>
       </c>
       <c r="B9">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>952</v>
+        <v>3577</v>
       </c>
       <c r="B10">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>3577</v>
-      </c>
-      <c r="B11">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excercise-NotView: Finishing with the practice succesfully (Note: Remember uncheck the Headers)
</commit_message>
<xml_diff>
--- a/DataTable manipulation/Sample Columns - Notview.xlsx
+++ b/DataTable manipulation/Sample Columns - Notview.xlsx
@@ -1,87 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF39D8-8D78-4570-9D89-82DB4CF05461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="6585" yWindow="2790" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+<x:workbook xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D30BCF6-CEB0-40A1-A3F4-60AAD4043DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-20610" yWindow="4485" windowWidth="20730" windowHeight="11760" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,103 +397,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>3359</v>
-      </c>
-      <c r="B1">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>9072</v>
-      </c>
-      <c r="B2">
-        <v>8996</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>623</v>
-      </c>
-      <c r="B3">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>324</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6643</v>
-      </c>
-      <c r="B5">
-        <v>88942</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3213</v>
-      </c>
-      <c r="B7">
-        <v>4324</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7732</v>
-      </c>
-      <c r="B8">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>952</v>
-      </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3577</v>
-      </c>
-      <c r="B10">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C11"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <x:selection activeCell="C1" sqref="C1 C:C"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="11.995781" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="0" t="n">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="n">
+        <x:v>195</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="n">
+        <x:v>3359</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="n">
+        <x:v>3394</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="n">
+        <x:v>9072</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
+        <x:v>8996</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="n">
+        <x:v>18068</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="0" t="n">
+        <x:v>623</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>679</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="0" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="C5" s="1" t="n">
+        <x:v>335</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="0" t="n">
+        <x:v>6643</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>88942</x:v>
+      </x:c>
+      <x:c r="C6" s="1" t="n">
+        <x:v>95585</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C7" s="1" t="n">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="0" t="n">
+        <x:v>3213</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="n">
+        <x:v>4324</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
+        <x:v>7537</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="0" t="n">
+        <x:v>7732</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
+        <x:v>7775</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="0" t="n">
+        <x:v>952</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="n">
+        <x:v>965</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="0" t="n">
+        <x:v>3577</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="n">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>3668</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>